<commit_message>
Farg'ona va Surxondaryo doklad oxirgi variant
</commit_message>
<xml_diff>
--- a/fergana_indeks_2022_07.xlsx
+++ b/fergana_indeks_2022_07.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\j.usmonov\Desktop\consumer_sentiment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DAB551-3958-44C3-B28C-3FD38F487682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E73692C-46BF-48CD-8A19-B0D24355C15D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="90" windowWidth="11430" windowHeight="13515" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12555" yWindow="510" windowWidth="13770" windowHeight="14055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -2007,10 +2007,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,403 +2085,403 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="C3">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="D3">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E3">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="F3">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G3">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="H3">
-        <v>138</v>
+        <v>165</v>
       </c>
       <c r="I3">
-        <v>152</v>
+        <v>168</v>
       </c>
       <c r="J3">
-        <v>149</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B4">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="C4">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="D4">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="E4">
-        <v>90</v>
+        <v>149</v>
       </c>
       <c r="F4">
-        <v>106</v>
+        <v>144</v>
       </c>
       <c r="G4">
-        <v>135</v>
+        <v>165</v>
       </c>
       <c r="H4">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="I4">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="J4">
-        <v>142</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C5">
-        <v>139</v>
+        <v>121</v>
       </c>
       <c r="D5">
-        <v>134</v>
+        <v>158</v>
       </c>
       <c r="E5">
-        <v>74</v>
+        <v>117</v>
       </c>
       <c r="F5">
-        <v>116</v>
+        <v>132</v>
       </c>
       <c r="G5">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H5">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="I5">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="J5">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C6">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="D6">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="E6">
-        <v>106</v>
+        <v>142</v>
       </c>
       <c r="F6">
-        <v>121</v>
+        <v>137</v>
       </c>
       <c r="G6">
         <v>158</v>
       </c>
       <c r="H6">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I6">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="J6">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B7">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C7">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="D7">
+        <v>135</v>
+      </c>
+      <c r="E7">
+        <v>133</v>
+      </c>
+      <c r="F7">
+        <v>130</v>
+      </c>
+      <c r="G7">
+        <v>162</v>
+      </c>
+      <c r="H7">
+        <v>142</v>
+      </c>
+      <c r="I7">
+        <v>145</v>
+      </c>
+      <c r="J7">
         <v>150</v>
-      </c>
-      <c r="E7">
-        <v>92</v>
-      </c>
-      <c r="F7">
-        <v>120</v>
-      </c>
-      <c r="G7">
-        <v>164</v>
-      </c>
-      <c r="H7">
-        <v>151</v>
-      </c>
-      <c r="I7">
-        <v>157</v>
-      </c>
-      <c r="J7">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8">
-        <v>128</v>
+        <v>139</v>
       </c>
       <c r="C8">
-        <v>115</v>
+        <v>139</v>
       </c>
       <c r="D8">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="E8">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="F8">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="G8">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="H8">
-        <v>133</v>
+        <v>170</v>
       </c>
       <c r="I8">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="J8">
-        <v>143</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9">
-        <v>128</v>
+        <v>138</v>
       </c>
       <c r="C9">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="D9">
-        <v>128</v>
+        <v>150</v>
       </c>
       <c r="E9">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="F9">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G9">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H9">
-        <v>111</v>
+        <v>151</v>
       </c>
       <c r="I9">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="J9">
-        <v>133</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B10">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C10">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="D10">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E10">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F10">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G10">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H10">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="I10">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="J10">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B11">
-        <v>123</v>
+        <v>137</v>
       </c>
       <c r="C11">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="D11">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E11">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="F11">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="G11">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="H11">
+        <v>137</v>
+      </c>
+      <c r="I11">
         <v>133</v>
       </c>
-      <c r="I11">
-        <v>126</v>
-      </c>
       <c r="J11">
-        <v>137</v>
+        <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B12">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C12">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="D12">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E12">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="F12">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G12">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H12">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="I12">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J12">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B13">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C13">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D13">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="E13">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="F13">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="G13">
         <v>165</v>
       </c>
       <c r="H13">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="I13">
-        <v>151</v>
+        <v>122</v>
       </c>
       <c r="J13">
-        <v>151</v>
+        <v>135</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B14">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C14">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D14">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="E14">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F14">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G14">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="H14">
-        <v>135</v>
+        <v>147</v>
       </c>
       <c r="I14">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="J14">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B15">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C15">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D15">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="E15">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F15">
         <v>120</v>
@@ -2490,208 +2490,211 @@
         <v>156</v>
       </c>
       <c r="H15">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="I15">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="J15">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B16">
+        <v>128</v>
+      </c>
+      <c r="C16">
+        <v>115</v>
+      </c>
+      <c r="D16">
+        <v>131</v>
+      </c>
+      <c r="E16">
+        <v>95</v>
+      </c>
+      <c r="F16">
+        <v>114</v>
+      </c>
+      <c r="G16">
+        <v>150</v>
+      </c>
+      <c r="H16">
         <v>133</v>
       </c>
-      <c r="C16">
-        <v>133</v>
-      </c>
-      <c r="D16">
-        <v>139</v>
-      </c>
-      <c r="E16">
-        <v>122</v>
-      </c>
-      <c r="F16">
-        <v>131</v>
-      </c>
-      <c r="G16">
-        <v>165</v>
-      </c>
-      <c r="H16">
-        <v>117</v>
-      </c>
       <c r="I16">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="J16">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="C17">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="D17">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="E17">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="F17">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="G17">
-        <v>179</v>
+        <v>166</v>
       </c>
       <c r="H17">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="I17">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="J17">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B18">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="C18">
+        <v>103</v>
+      </c>
+      <c r="D18">
+        <v>126</v>
+      </c>
+      <c r="E18">
+        <v>90</v>
+      </c>
+      <c r="F18">
+        <v>106</v>
+      </c>
+      <c r="G18">
+        <v>135</v>
+      </c>
+      <c r="H18">
         <v>136</v>
       </c>
-      <c r="D18">
-        <v>140</v>
-      </c>
-      <c r="E18">
-        <v>124</v>
-      </c>
-      <c r="F18">
-        <v>133</v>
-      </c>
-      <c r="G18">
-        <v>185</v>
-      </c>
-      <c r="H18">
-        <v>165</v>
-      </c>
       <c r="I18">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="J18">
-        <v>173</v>
+        <v>142</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="C19">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D19">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="E19">
+        <v>88</v>
+      </c>
+      <c r="F19">
+        <v>110</v>
+      </c>
+      <c r="G19">
+        <v>152</v>
+      </c>
+      <c r="H19">
         <v>133</v>
       </c>
-      <c r="F19">
-        <v>130</v>
-      </c>
-      <c r="G19">
-        <v>162</v>
-      </c>
-      <c r="H19">
-        <v>142</v>
-      </c>
       <c r="I19">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="J19">
-        <v>150</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B20">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="C20">
+        <v>118</v>
+      </c>
+      <c r="D20">
+        <v>121</v>
+      </c>
+      <c r="E20">
+        <v>86</v>
+      </c>
+      <c r="F20">
+        <v>108</v>
+      </c>
+      <c r="G20">
+        <v>179</v>
+      </c>
+      <c r="H20">
+        <v>104</v>
+      </c>
+      <c r="I20">
+        <v>109</v>
+      </c>
+      <c r="J20">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>136</v>
+      </c>
+      <c r="C22">
+        <v>124</v>
+      </c>
+      <c r="D22">
+        <v>135</v>
+      </c>
+      <c r="E22">
         <v>112</v>
       </c>
-      <c r="D20">
-        <v>133</v>
-      </c>
-      <c r="E20">
+      <c r="F22">
+        <v>124</v>
+      </c>
+      <c r="G22">
+        <v>161</v>
+      </c>
+      <c r="H22">
+        <v>140</v>
+      </c>
+      <c r="I22">
         <v>143</v>
       </c>
-      <c r="F20">
-        <v>129</v>
-      </c>
-      <c r="G20">
-        <v>166</v>
-      </c>
-      <c r="H20">
-        <v>137</v>
-      </c>
-      <c r="I20">
-        <v>133</v>
-      </c>
-      <c r="J20">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21">
-        <v>136</v>
-      </c>
-      <c r="C21">
-        <v>124</v>
-      </c>
-      <c r="D21">
-        <v>135</v>
-      </c>
-      <c r="E21">
-        <v>112</v>
-      </c>
-      <c r="F21">
-        <v>124</v>
-      </c>
-      <c r="G21">
-        <v>161</v>
-      </c>
-      <c r="H21">
-        <v>140</v>
-      </c>
-      <c r="I21">
-        <v>143</v>
-      </c>
-      <c r="J21">
+      <c r="J22">
         <v>148</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J20">
+    <sortCondition descending="1" ref="B2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -2822,8 +2825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AI21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" activeCellId="1" sqref="A5:XFD5 A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>